<commit_message>
Added feature for retrieving existing customer record
</commit_message>
<xml_diff>
--- a/quotation_tracking.xlsx
+++ b/quotation_tracking.xlsx
@@ -5,16 +5,17 @@
   <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Google Drive\Personal\UiPath\Creating Quotation\Creating Quotations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Google Drive\Personal\UiPath\Creating Quotation\Automate Quotation Creation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F4FF5D-CCCC-4402-99F3-9E4E36EBDD5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BFA6B6-6FB4-47AE-97B1-59DE2561A29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="2205" yWindow="2355" windowWidth="25110" windowHeight="15345" firstSheet="0" activeTab="0" xr2:uid="{722A32AC-850B-46C6-AEDC-5E73FC0CCF17}"/>
+    <x:workbookView xWindow="660" yWindow="2040" windowWidth="23640" windowHeight="15345" firstSheet="0" activeTab="2" xr2:uid="{722A32AC-850B-46C6-AEDC-5E73FC0CCF17}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="quotation tracking" sheetId="2" r:id="rId1"/>
-    <x:sheet name="Counter" sheetId="3" r:id="rId2"/>
+    <x:sheet name="customer list" sheetId="4" r:id="rId2"/>
+    <x:sheet name="Config file" sheetId="3" r:id="rId3"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="191029"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <x:si>
     <x:t>Quotation#</x:t>
   </x:si>
@@ -68,13 +69,118 @@
     <x:t>Prepared by</x:t>
   </x:si>
   <x:si>
-    <x:t>Quote_#0</x:t>
-  </x:si>
-  <x:si>
     <x:t>Quote_#1</x:t>
   </x:si>
   <x:si>
-    <x:t>2</x:t>
+    <x:t>4/6/2021</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30 days</x:t>
+  </x:si>
+  <x:si>
+    <x:t>John Doe</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JohnDoe Pte Ltd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Orchard Road 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>711 222</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6111 2222</x:t>
+  </x:si>
+  <x:si>
+    <x:t>JohnDoe@JD.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bolt</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Quote_#2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Richard Roe</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RR Marketing Pte Ltd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Marina Bay 2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>722 333</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6222 3333</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Richard@RR.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Quote_#3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Isabelle Tan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ITS digital art pte ltd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ang Mo Kio Industrial Park A2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>744 555</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6444 5555</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Isatan@ITS.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>King</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Quote_#4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>May Tan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MT Technologies Pte Ltd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Jurong Industrial Park</x:t>
+  </x:si>
+  <x:si>
+    <x:t>755 666</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6555 6666</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MayTan@MTech.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Shaun Neo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Customer ID</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cust_#1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cust_#2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cust_#3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cust_#4</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -117,7 +223,7 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="5">
+  <x:cellStyleXfs count="19">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
@@ -126,6 +232,48 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="1" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -467,10 +615,10 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:L16"/>
+  <x:dimension ref="A1:L4"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="B4" sqref="B4 B4:B4"/>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="F13" sqref="F13 F13:F13"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,70 +666,133 @@
       <x:c r="A2" s="5" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="J2" s="4" t="s"/>
+      <x:c r="B2" s="4" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C2" s="4" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D2" s="4" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E2" s="4" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F2" s="4" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="G2" s="4" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H2" s="4" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="I2" s="4" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="J2" s="4" t="s">
+        <x:v>19</x:v>
+      </x:c>
       <x:c r="L2" s="6" t="s"/>
     </x:row>
     <x:row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A3" s="5" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B3" s="4" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="B3" s="4" t="s"/>
-      <x:c r="C3" s="4" t="s"/>
-      <x:c r="D3" s="4" t="s"/>
-      <x:c r="E3" s="4" t="s"/>
-      <x:c r="F3" s="4" t="s"/>
-      <x:c r="G3" s="4" t="s"/>
-      <x:c r="H3" s="4" t="s"/>
-      <x:c r="I3" s="4" t="s"/>
-      <x:c r="J3" s="4" t="s"/>
+      <x:c r="C3" s="4" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D3" s="4" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="E3" s="4" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="F3" s="4" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="G3" s="4" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="H3" s="4" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="I3" s="4" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="J3" s="4" t="s">
+        <x:v>19</x:v>
+      </x:c>
     </x:row>
     <x:row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="5" t="s"/>
-      <x:c r="B4" s="4" t="s"/>
-      <x:c r="C4" s="4" t="s"/>
-      <x:c r="D4" s="4" t="s"/>
-      <x:c r="E4" s="4" t="s"/>
-      <x:c r="F4" s="4" t="s"/>
-      <x:c r="G4" s="4" t="s"/>
-      <x:c r="H4" s="4" t="s"/>
-      <x:c r="I4" s="4" t="s"/>
-      <x:c r="J4" s="4" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="5" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="5" t="s"/>
-    </x:row>
-    <x:row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <x:c r="A7" s="5" t="s"/>
-    </x:row>
-    <x:row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <x:c r="A8" s="5" t="s"/>
-    </x:row>
-    <x:row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <x:c r="A9" s="5" t="s"/>
-    </x:row>
-    <x:row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <x:c r="A10" s="5" t="s"/>
-    </x:row>
-    <x:row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <x:c r="A11" s="5" t="s"/>
-    </x:row>
-    <x:row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <x:c r="A12" s="5" t="s"/>
-    </x:row>
-    <x:row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <x:c r="A13" s="5" t="s"/>
-    </x:row>
-    <x:row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <x:c r="A14" s="5" t="s"/>
-    </x:row>
-    <x:row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <x:c r="A15" s="5" t="s"/>
-    </x:row>
-    <x:row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <x:c r="A16" s="5" t="s"/>
+      <x:c r="A4" s="5" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B4" s="4" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C4" s="4" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D4" s="4" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="E4" s="4" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="F4" s="4" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="G4" s="4" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="H4" s="4" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="I4" s="4" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="J4" s="4" t="s">
+        <x:v>34</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:12">
+      <x:c r="A5" s="4" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="B5" s="4" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C5" s="4" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D5" s="4" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="E5" s="4" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="F5" s="4" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="G5" s="4" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="H5" s="4" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="I5" s="4" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="J5" s="4" t="s">
+        <x:v>42</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:12">
+      <x:c r="F13" s="4" t="s"/>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -593,24 +804,181 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{1740D2E5-429E-4E75-9BA8-1228ABFEC812}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:G1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0">
+      <x:selection activeCell="A5" sqref="A5 A5:A5 A2:G5"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="18.710938" style="4" customWidth="1"/>
+    <x:col min="2" max="7" width="23" style="4" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="4" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="B1" s="4" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="C1" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="D1" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="E1" s="4" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="F1" s="4" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="G1" s="4" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:7">
+      <x:c r="A2" s="4" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="B2" s="4" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C2" s="4" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D2" s="4" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="E2" s="4" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="F2" s="4" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G2" s="4" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:7">
+      <x:c r="A3" s="4" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B3" s="4" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C3" s="4" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="D3" s="4" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="E3" s="4" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="F3" s="4" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="G3" s="4" t="s">
+        <x:v>26</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:7">
+      <x:c r="A4" s="4" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="B4" s="4" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C4" s="4" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="D4" s="4" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="E4" s="4" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="F4" s="4" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="G4" s="4" t="s">
+        <x:v>33</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:7">
+      <x:c r="A5" s="4" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="B5" s="4" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="C5" s="4" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="D5" s="4" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="E5" s="4" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="F5" s="4" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="G5" s="4" t="s">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:7">
+      <x:c r="A6" s="4" t="s"/>
+      <x:c r="B6" s="4" t="s"/>
+      <x:c r="C6" s="4" t="s"/>
+      <x:c r="D6" s="4" t="s"/>
+      <x:c r="E6" s="4" t="s"/>
+      <x:c r="F6" s="4" t="s"/>
+      <x:c r="G6" s="4" t="s"/>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{DBAA147B-1A31-49A6-A3A3-F6C2F7180AF0}" mc:Ignorable="x14ac xr xr2 xr3">
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1"/>
+  <x:dimension ref="A1:B2"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
-      <x:selection activeCell="F8" sqref="F8 F8:F8"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="H33" sqref="H33 H33:H33"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:sheetData>
-    <x:row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="4" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:6"/>
+    <x:row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="4" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B1" s="4" t="n">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="4" t="s"/>
+      <x:c r="B2" s="4" t="s"/>
+    </x:row>
+    <x:row r="33" spans="1:8"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>